<commit_message>
subgroup analysis & Funnel plot
subgroup analysis& Funnel plot are now added!
</commit_message>
<xml_diff>
--- a/static/analysis_mean.xlsx
+++ b/static/analysis_mean.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mirzafarangi/Desktop/meta-analysis/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alenka/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CCD4AAFF-EA02-E443-9F07-D5B0BE74B9CE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8D9D0E-B04C-FE42-B8E0-9B073FE87974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15940" xr2:uid="{705A08C2-2E62-1C47-B8E8-4A0A1A64469E}"/>
   </bookViews>
@@ -25,41 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Study</t>
   </si>
   <si>
-    <t>Bisch 2017</t>
-  </si>
-  <si>
-    <t>Corbisiero 2017</t>
-  </si>
-  <si>
-    <t>Irastorza 2016</t>
-  </si>
-  <si>
-    <t>Miller 2015</t>
-  </si>
-  <si>
-    <t>Mitchell 2012</t>
-  </si>
-  <si>
-    <t>Rapport 2012</t>
-  </si>
-  <si>
-    <t>Reimherr 2015</t>
-  </si>
-  <si>
-    <t>Richard-Lepouriel 2015</t>
-  </si>
-  <si>
-    <t>Skirrow &amp; Asherson</t>
-  </si>
-  <si>
-    <t>Surman 2015</t>
-  </si>
-  <si>
     <t>N1</t>
   </si>
   <si>
@@ -79,6 +49,48 @@
   </si>
   <si>
     <t>Moderator</t>
+  </si>
+  <si>
+    <t>subgroup</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>subgroup1</t>
+  </si>
+  <si>
+    <t>subgroup2</t>
+  </si>
+  <si>
+    <t>subgroup3</t>
   </si>
 </sst>
 </file>
@@ -101,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,6 +144,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -158,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -175,9 +193,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -193,7 +214,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -489,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C58B5C-33BD-E34D-8BAE-1C3085D4B7ED}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,38 +526,42 @@
     <col min="6" max="6" width="29.5" style="2" customWidth="1"/>
     <col min="7" max="7" width="29.6640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="19.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="18.33203125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2">
         <v>23</v>
@@ -557,12 +582,15 @@
         <v>3.3</v>
       </c>
       <c r="H2" s="2">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>47</v>
@@ -583,12 +611,15 @@
         <v>3.1</v>
       </c>
       <c r="H3" s="2">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <v>44</v>
@@ -609,12 +640,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="H4" s="2">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>78</v>
@@ -635,12 +669,15 @@
         <v>2.5</v>
       </c>
       <c r="H5" s="2">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2">
         <v>311</v>
@@ -661,12 +698,15 @@
         <v>6.1</v>
       </c>
       <c r="H6" s="2">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2">
         <v>144</v>
@@ -687,12 +727,15 @@
         <v>4.2</v>
       </c>
       <c r="H7" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
         <v>79</v>
@@ -713,12 +756,15 @@
         <v>4.3</v>
       </c>
       <c r="H8" s="2">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2">
         <v>59</v>
@@ -739,12 +785,15 @@
         <v>2.1</v>
       </c>
       <c r="H9" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2">
         <v>214</v>
@@ -765,12 +814,15 @@
         <v>2.5</v>
       </c>
       <c r="H10" s="2">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2">
         <v>110</v>
@@ -791,7 +843,10 @@
         <v>5.6</v>
       </c>
       <c r="H11" s="2">
-        <v>75</v>
+        <v>42</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
funnel fix scale fig
</commit_message>
<xml_diff>
--- a/static/analysis_mean.xlsx
+++ b/static/analysis_mean.xlsx
@@ -8,17 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alenka/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8D9D0E-B04C-FE42-B8E0-9B073FE87974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CE92F9-B42F-1C41-92DA-C6D28A17478A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15940" xr2:uid="{705A08C2-2E62-1C47-B8E8-4A0A1A64469E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -510,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C58B5C-33BD-E34D-8BAE-1C3085D4B7ED}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,7 +536,7 @@
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -587,8 +593,12 @@
       <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="2">
+        <f>F2-C2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -614,10 +624,14 @@
         <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J11" si="0">F3-C3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -645,8 +659,12 @@
       <c r="I4" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -674,8 +692,12 @@
       <c r="I5" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -701,10 +723,14 @@
         <v>51</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -730,10 +756,14 @@
         <v>41</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -761,8 +791,12 @@
       <c r="I8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -788,10 +822,14 @@
         <v>29</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -817,10 +855,14 @@
         <v>38</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -846,7 +888,11 @@
         <v>42</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>